<commit_message>
Control de asistencia de Abraham
</commit_message>
<xml_diff>
--- a/Control de asistencia.xlsx
+++ b/Control de asistencia.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\DocenciaPostDoc\R_CEINDO\Github\R_course_ceindo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R_course_ceindo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EDD319B-778D-4AE8-B1F7-A03469AB679E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B4FE7A-B922-4E92-AC71-0E1259B9118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="2070" windowWidth="26655" windowHeight="26820" xr2:uid="{02895637-79F9-4548-9763-73B60EB026D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02895637-79F9-4548-9763-73B60EB026D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,158 +35,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>E-mail</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marta Sala Climent </t>
   </si>
   <si>
-    <t>MARTA.SALA1@alumnos.uchceu.es</t>
-  </si>
-  <si>
     <t>Marina Toquero</t>
   </si>
   <si>
-    <t>marinatc112@gmail.com</t>
-  </si>
-  <si>
     <t>Gemma María García Lluch</t>
   </si>
   <si>
-    <t>gemma.garcia2@alumnos.uchceu.es</t>
-  </si>
-  <si>
-    <t>belvicmig@alumnos.uchceu.es</t>
-  </si>
-  <si>
     <t>Miguel Ángel Beltrán Viciano</t>
   </si>
   <si>
     <t>Alba Couto Rodríguez</t>
   </si>
   <si>
-    <t>alba.coutorodriguez1@usp.ceu.es</t>
-  </si>
-  <si>
-    <t>m.quiralte@usp.ceu.es</t>
-  </si>
-  <si>
     <t>Quiralte Pulido, Miguel</t>
   </si>
   <si>
     <t>Antonio Tarín Pelló</t>
   </si>
   <si>
-    <t>antonio.tarin@alumnos.uchceu.es</t>
-  </si>
-  <si>
-    <t>sandra.camunasalberca@ceu.es</t>
-  </si>
-  <si>
     <t>Sandra M. Camuñas Alberca</t>
   </si>
   <si>
-    <t>maria.bajofernandez1@ceu.es</t>
-  </si>
-  <si>
     <t>María Bajo Fernández</t>
   </si>
   <si>
-    <t>l.mayo1@usp.ceu.es</t>
-  </si>
-  <si>
     <t>Laura Mayo Martinez</t>
   </si>
   <si>
-    <t>david.chamososanchez@usp.ceu.es</t>
-  </si>
-  <si>
     <t>David Chamoso Sanchez</t>
   </si>
   <si>
-    <t>pau.cuevas.ce@ceindo.ceu.es</t>
-  </si>
-  <si>
     <t>Paula Cuevas Delgado</t>
   </si>
   <si>
-    <t>m.moran4@usp.ceu.es</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maria Moran Garrido </t>
   </si>
   <si>
-    <t>belenfernandezrequena@gmail.com</t>
-  </si>
-  <si>
     <t>Belén Fdez Requena</t>
   </si>
   <si>
     <t>Carla Palacios Gorba</t>
   </si>
   <si>
-    <t>carla.palaciosgorba@uchceu.es</t>
-  </si>
-  <si>
     <t>Sara Martínez López</t>
   </si>
   <si>
-    <t>sara.martinezlopez@ceu.es</t>
-  </si>
-  <si>
-    <t>samantha.moratalmartinez@uchceu.es</t>
-  </si>
-  <si>
-    <t>Samantha Moratal Martínez</t>
-  </si>
-  <si>
-    <t>jaime.jordanlopez1@uchceu.es</t>
-  </si>
-  <si>
     <t>Jaime Jordán López</t>
   </si>
   <si>
-    <t>elena.bocoscorredor1@usp.ceu.es</t>
-  </si>
-  <si>
     <t>Elena Bocos Corredor</t>
   </si>
   <si>
     <t xml:space="preserve">Ignacio Piédrola Pedraza </t>
   </si>
   <si>
-    <t>i.piedrola@usp.ceu.es</t>
-  </si>
-  <si>
-    <t>Sandra Camuñas Alberca</t>
-  </si>
-  <si>
-    <t>marion.toquet1@uchceu.es</t>
-  </si>
-  <si>
     <t>Marion Toquet</t>
   </si>
   <si>
-    <t>yuval.markovich@uchceu.es</t>
-  </si>
-  <si>
-    <t>Yuval Markovich</t>
-  </si>
-  <si>
     <t>Javier Arranz Herrero</t>
   </si>
   <si>
-    <t>pepepneumo@gmail.com</t>
-  </si>
-  <si>
-    <t>j.arranz3@usp.ceu.es</t>
-  </si>
-  <si>
     <t>Jose ramon cugat garcia</t>
   </si>
   <si>
@@ -208,6 +125,12 @@
   </si>
   <si>
     <t>Sesión 7</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Alba Espi</t>
   </si>
 </sst>
 </file>
@@ -567,255 +490,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C7B028-3BAD-4BE0-BA17-90D4CD178BC1}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mistakes and assistance list
</commit_message>
<xml_diff>
--- a/Control de asistencia.xlsx
+++ b/Control de asistencia.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R_course_ceindo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto.gildelafuent\Desktop\alberto\repos_git\R_course_ceindo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B4FE7A-B922-4E92-AC71-0E1259B9118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1316F6-D7AE-4AE2-A599-5AB7E2089F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02895637-79F9-4548-9763-73B60EB026D3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{02895637-79F9-4548-9763-73B60EB026D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -493,17 +492,17 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="1.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,12 +528,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -545,7 +544,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -553,7 +552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -563,8 +562,11 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -574,8 +576,11 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -585,13 +590,16 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -601,8 +609,11 @@
       <c r="D9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -612,8 +623,11 @@
       <c r="D10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -623,8 +637,11 @@
       <c r="D11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -634,8 +651,11 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -645,8 +665,11 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -656,8 +679,11 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -667,8 +693,11 @@
       <c r="D15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -678,8 +707,11 @@
       <c r="D16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -689,8 +721,11 @@
       <c r="D17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -700,8 +735,11 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -711,8 +749,11 @@
       <c r="D19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -722,8 +763,11 @@
       <c r="D20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -733,16 +777,22 @@
       <c r="D21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -752,8 +802,11 @@
       <c r="D23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -761,6 +814,9 @@
         <v>30</v>
       </c>
       <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>